<commit_message>
Get daily reddit data: Tue Mar 25 08:11:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_30.xlsx
+++ b/data/collected_data/2025_03_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C513"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3610 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1jje7fn</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Throwback ombre set Sydney 2020</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jje7fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1jjdqqc</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>They remind me of an almond. They are so cute</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a96n8rbesqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1jjczqw</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Tips with what polish?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z60qfr74sqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1jjdcbb</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Fresh new set!! What do you think?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjdcbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1jjcbpk</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>I’m back to short almonds 🤍</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8si90a0pvrqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1jjc9sd</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Florals for my Current Set</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjc9sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1jjbnal</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷💐</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ila17sannrqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1jjbcc6</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>14K butterfly nailzzz</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjbcc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1jj9ofa</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Please help me</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj9ofa</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1jjaq4c</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>do these look like ?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysdx8qkxdrqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1jjah7r</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Cateye is back</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cppofoffbrqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1jj9s1t</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Trying to grow my nails after years of hand eczema and nail biting</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj9s1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1jja2td</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Sparkles!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gt1r0si7rqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1jj9xuc</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Easter colors 🐣</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj9xuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1jj9vjl</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj9vjl/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1jj94xv</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>10th wedding anniversary nails. Kept it simple: cat eye gel &amp; bows. 💕🎀</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k99m9b8iyqqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1jj8uwr</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Making a Lilo &amp; Stitch Nail Set starting with a lil 3d Surfboard</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hvxwx18yvqqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1jj8k1s</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>New nails 💖</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj8k1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1jj8bt5</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Squoval Nails ?🌼</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj8bt5/squoval_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1jj4h4a</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>longest my nails have ever grown &amp; i feel so glam 🤩</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj4h4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1jj6vr5</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>What should I use to help my pinkie nails grow longer?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lp3zsogoeqqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1jj5xvf</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Do y'all need to sharpen your acrylic nails every so often?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj5xvf/do_yall_need_to_sharpen_your_acrylic_nails_every/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1jj4ue9</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>First time getting cat eye, but do  they look tacky?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/72k7bkraypqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1jj6yoh</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Onycholysis Question?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj6yoh/onycholysis_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1jj73kb</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Unhappy with dip removal at salon</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj73kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1jj6qre</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>My girlfriend does her own nails</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj6qre</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1jj77by</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>First time using/applying gel-x</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj77by</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1jj6dxa</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Some “stain glass” style nails I did on my friend</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tiqe3bchaqqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1jj5o6d</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Got spoiled by my bf and his sister today 🥰</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj5o6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1jj5avu</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Pastel rainbow with chrome</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hkci5fs1qqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1jj4yh9</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Bubbling on clear builder gel</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj4yh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1jj4q6v</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Greek Tiles (by the pool)</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6mxbgihxpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1jj4ogo</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Chrome + magnetic effect. Not bad for Walmart press-ons!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj4ogo</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1jj4ldg</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtg5iszhwpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1jj4fu8</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Tips for keeping glue on nails on??</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj4fu8/tips_for_keeping_glue_on_nails_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1jj4egi</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>How can I shift the hyponychium, and make the free edge shorter?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj4egi</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1jj4eze</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Press ons 😊</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj4eze</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1jj4erd</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Sistaco flamingo</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj4erd</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1jj46ot</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Is there something like a wax resist to prevent getting polish/airbrush on your skin?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj46ot/is_there_something_like_a_wax_resist_to_prevent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1jj43y2</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj43y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1jj41sm</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>my gel x nail came off😭 what should i do</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj41sm/my_gel_x_nail_came_off_what_should_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1jj40ds</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Paid $75 for this…was I overcharged?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/logicmh3spqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1jj3wqx</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Dark nails on a dark skirt &lt;3</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft24ugxarpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1jj3s53</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>just tried to pick up my laptop 🫠</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd5gztbdqpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1jj3rdb</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Vertical split nails, help.</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj3rdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1jj39h0</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Builder Gel lifting</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj39h0/builder_gel_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1jj35e6</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Warm Natural Pink 🌷</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqb8haiglpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1jj30tl</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>What are these white smudges on my nails?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfctjk7rkpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1jj2eeh</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Press on help</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2ij1xx5gpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1jj3203</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Bubble buddy from spongebob  nails i made for Vday🫧💕</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj3203</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1jj2ze0</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Salmon Chrome gel on natural nails !</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwwd4vngkpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1jj2wan</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>More dots</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf9eumdtjpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1jj2vkp</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Cat Eye Gel Bulking Help</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj2vkp/cat_eye_gel_bulking_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1jj2rm1</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>March manicure 🍃</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhbv4v9uipqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1jj2olc</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Is this nude too nude?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj2olc</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1jj1z07</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>How often to give nails a break?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj1z07/how_often_to_give_nails_a_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1jj0r8x</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>What am i doing wrong</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj0r8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1jj15pf</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>what can i do to "hide" the growth? SOS</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3v0uam97pqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1jj14j1</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Did these myself and I don’t care if there to long 😬</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/evyz1y407pqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1jj0zt9</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Sponge with different shades, dabbing on the nail mani</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj0zt9/sponge_with_different_shades_dabbing_on_the_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1jj0y0g</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My nails are freshly done, what you girls think?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj0y0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1jj0w36</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Better cheaper alternative to acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jj0w36/better_cheaper_alternative_to_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1jj0vb3</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Made use out of some random nail charms 🍬</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ygcsu3q85pqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1jj0mf7</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Tales from a Picker...anyone else?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaje7rmk3pqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1jj0ghs</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Sakura spring set 🌸</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj0ghs</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1jj0db3</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I took a better pic</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwlvaawu1pqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1jj0c1p</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Did my nails 🤎⭐️</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06vfsquk1pqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1jj0bg5</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>New set 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj0bg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1jj06mg</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Aurora Chrome Cat Eye</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dhwwgu4l0pqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1jj06or</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>tried black for the first time</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zd30a0ul0pqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1jiz9q2</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Mani frequency when trying to heal nails</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0ceh0h6uoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1jiza13</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Fruit and veggie nails for National Nutrition Month!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiza13</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1jj00p7</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>New Nails Monday</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj00p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1jiz4wz</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>First time trying out rhinestones</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9m9pqwk8toqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1jiz2s4</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Back to doing my own dip nails!</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo5jrlvssoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1jiz199</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>How does this design look?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru2z2cehsoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1jiz04g</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Pink pedi</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiz04g</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1jiyruf</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>I love chrome nails 🩷</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0x3zkynqoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1jiypcb</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Shaping and help with the lumps?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiypcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1jixxmf</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>First set</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jixxmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1jixrzg</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I love this combo, don’t you?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s96qaiqjoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1jixe4s</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Any tips to help my nails grow?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0orc3z3hoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1jixc08</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Nail Reformation press-ons have endured a week-long vacation</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwwjqq3pgoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1jix9pb</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Green nails!!</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jix9pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1jix9b0</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Happy nails</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulfek8f7goqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1jix59r</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>the weather is bright but my nails stay gloomy</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jix59r</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1jix2qt</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>I’m obsessed with this set</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pewln3czeoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1jiwwyv</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Springtime nails! Love the 3d elements - I don't use them nearly enough</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed4ok3yudoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1jiwn3q</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Nail Strengthening</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jiwn3q/nail_strengthening/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1jiwh4p</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Spring leaves feat. little bug friends!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiwh4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1jiwb2b</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Tragic 💀</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep3ctzdk9oqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1jiwa85</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Mermaid chrome 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiwa85</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1jiw0y2</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>these turned out so cute!! it was a lot of fun making the squiggles</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jx9p4x0j7oqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1jivr5g</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>What is happening with my nails?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jivr5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1jivu6f</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Cybergoth inspired nails!</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jivu6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1jivsfp</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Can you guess my favorite color???</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jivsfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1jivsaf</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Pretty milky white nails my friend made &amp; I decorated</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jivsaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1jive6w</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>I just got acrylics for the first time and am finding tasks very difficult. Should I get them removed or try to learn how to use them?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jive6w/i_just_got_acrylics_for_the_first_time_and_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1jivbz9</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>vote for green ✓ edgy or not?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jivbz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1jii8rs</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Helping damaged nails: suggestions</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyk5o0acakqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1jjcglo</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Japanese polish: Canmake N97 Puddle</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bgebxxexrqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1jjc6vt</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Thoughts? I want to like feel like these colors go together but I don't think they do but they kind of do but they kind of don't but like they feel good together but they don't like look right? I don't know</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50f3ct00urqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1jjafuh</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>My skills with my non dominate hand from a person who barely paints their nails.</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoqty5d1brqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1jj90j0</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Bold, single-tone polishes?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj90j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1jj8xrq</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>first attempt at both french and nail art, love how it came out 🐸🌸</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j9pucmsmwqqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1jj8vx7</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>My phone can’t handle the flakies at golden hour</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj8vx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1jj8qbn</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>this is your sign to try thermonuclear 🔥</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xm5adwksuqqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1jj8g2x</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Alien Invasion - Mooncat</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj8g2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1jj8bw0</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>loving this combo 💜</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj8bw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1jj8bhi</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Tiffany Blue, Anyone?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdqcx705rqqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1jj85on</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>BKL Change Often Feels Unpleasant</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj85on</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1jj7dx9</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Preferred gel brand?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj7dx9/preferred_gel_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1jj6m4b</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Aston Martin Racing Green(s)</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj6m4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1jj6k2h</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Gel base &amp; top coat questions</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj6k2h/gel_base_top_coat_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1jj6crv</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Polishes that you feel photos don’t do justice?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj6crv/polishes_that_you_feel_photos_dont_do_justice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1jj6bt9</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Felt girly this week</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj6bt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1jj6b54</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Longevity by brand - who lasts longest on you?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj6b54/longevity_by_brand_who_lasts_longest_on_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1jj66lo</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Favorite new combo</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uq48ygs8qqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1jj5znp</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Ultrahot</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj5znp</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1jj5riu</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Polish Pick Up Info</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj5riu/polish_pick_up_info/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1jj5l3f</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Layering is saving my no buy</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj5l3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1jj5b2i</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Looking for a shiftier version of this deep blue green</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5ctb3wt1qqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1jj56ip</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Vampy Red</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj56ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1jj56ez</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Vampy Red</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj56ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1jj5448</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Does this nail shape look good/fit me?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj5448</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1jj4jcb</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Help me pick a conference color!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo6krge2wpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1jj4etr</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Rock Candy</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qh3q28q3vpqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1jj43ej</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>I don’t usually share my mani, but I think this one turned out pretty rad.</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj43ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1jj37mr</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>What's your ideal bottle SIZE</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj37mr/whats_your_ideal_bottle_size/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1jj2lbu</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Turn out that capping/rolling your nails doesn't matter if you go bowling</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzmvm86ghpqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1jj2fum</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Spring nails for funsies 🌸</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ljl2jpfgpqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1jj20y3</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Does anyone know what happened to Kyle of Color Expression</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj20y3/does_anyone_know_what_happened_to_kyle_of_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1jj1xpw</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Princess nails 👑</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj1xpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1jj1fxl</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Top &amp; Base Coat Recommendations (for longevity)</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj1fxl/top_base_coat_recommendations_for_longevity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1jj0yxe</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Electric Blue but I hate it</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yeg1rox5pqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1jj0r7y</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>The Brutal Beauty of Deep Winter💜💙</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj0r7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1jj0mpm</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>every time i fill them in i’m tempted to leave them like this bc it looks so pretty and clean</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj0mpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1jj0hbt</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>When do sales happen for ILNP, MoonCat, Death Valley, Bees Knees?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jj0hbt/when_do_sales_happen_for_ilnp_mooncat_death/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1jizz08</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Hello Hawai’i Ya 💜</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2u0sz43zoqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1jiz5j0</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Spring has sprung - Blue &amp; white</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiz5j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1jiy0zp</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Anyone hear from Gracie Jay about Feb restock or receive theirs?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jiy0zp/anyone_hear_from_gracie_jay_about_feb_restock_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1jixg7e</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>What color do you like, but hate on your nails?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jixg7e/what_color_do_you_like_but_hate_on_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1jixdvp</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Spring is in bloom</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jixdvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1jiwc4d</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Ever get stuck on one polish?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jiwc4d/ever_get_stuck_on_one_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1jiw3xs</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Matte French</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ulrovsy7oqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1jiw1vp</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Jumped on the magnet bandwagon</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svcv73rl7oqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ji4c97</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Acrylics or gels better for stopping nail biting?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ji4c97/acrylics_or_gels_better_for_stopping_nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1jij7zt</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>ISO an indie polish, white or whitish with chunky blue or cobalt flakes. I’m a newbie to indie polish and missed Chamaeleon Polish’s Cortana. Any similar polishes come to mind?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jij7zt/iso_an_indie_polish_white_or_whitish_with_chunky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1jirwbq</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>The iconic MC - Sabertooth</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brok9tk8dnqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1jiv9et</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Progress since January 🥰</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiv9et</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1jiumx8</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Waylaid by Bullshit</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiumx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1jiumko</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Starrily cured my FOMO 🤩</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/evyx626ixnqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1jiucpb</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Help looking for a strong matte topcoat?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiucpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1jiu59f</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Another round of Atomic Sherbert by ILNP</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v048ohm4unqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1jitzuo</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Nails inc - new product?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymczryb5tnqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1jitl7n</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>De-influence Me from buying all these</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jitl7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1jitf66</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>When your polish accidentally matches your hair</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jitf66</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1jitbi4</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Anyone grab anything from Cirque's Glazed 2025 Jellies line?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jitbi4/anyone_grab_anything_from_cirques_glazed_2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1jit8nv</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Help with application</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jit8nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1jit21y</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Trouble finding this shade!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5khousr7mnqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1jit166</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Spring has sprung</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnyrbi31mnqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1jisu58</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Cream Cheese and Jelly Nails, inspired by my breakfast</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdrf4ebmknqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1jisd7u</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Base Coats to Prevent Staining?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jisd7u/base_coats_to_prevent_staining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1jis3ie</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Nail polish giving ick while pregnant?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jis3ie/nail_polish_giving_ick_while_pregnant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1jire5e</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>💚🩵Star Pond 2.0💙💜</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jire5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1jir4ny</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Lavender Sky is my new fave</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jir4ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1jiqs83</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I heard that you don’t need a water based topcoat for nail powder… just clear school glue.  Thrilled to report it works</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiqs83</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1jiqqxv</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>The reality of my manicure after a week of office work, washing a muddy dog multiple times, doing chores, rock climbing, and miscellaneous other activities (dog tax incl.)</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiqqxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1jip8wf</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>FINALLY found my perfect regular red! 🍒</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jip8wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1jip4vw</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Rosé all day</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jip4vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1jior40</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Show Me Your Favorite Color Club!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jior40/show_me_your_favorite_color_club/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1jionzl</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Not Orly! Sea you soon from Catrice</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxk8ajdpkmqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1jinc2a</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Celebrating the start of spring with a wildflower meadow 🌷</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jinc2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1jin4f2</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jin4f2/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1jin1vl</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Orly Off The Grid topped with Colores De Carol Lagoon</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r721z0zj1mqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1jimolv</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Roast my Future Mooncat Order</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jimolv</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1jjdb2f</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Studio Ghibli themed nails!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjdb2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1jjcfbf</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Spring Set</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iakghp4ywrqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1jjb6v1</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>14K Butterfly nailzzz</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjb6v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1jjanh0</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I love seeing the art and skill on this sub!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jjanh0/i_love_seeing_the_art_and_skill_on_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1jja8dz</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Recent practice</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jja8dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1jj9u2s</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Kill bill inspired set by me :)</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s5dimm55rqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1jj8v90</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Making a Lilo &amp; Stitch Nail Set starting with a lil 3d Surfboard</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bnh2abh1wqqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1jj8gyx</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>transparent nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj8gyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1jj856u</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Swipe for the inspo ✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj856u</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1jj84nr</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Spring Freestyle✨</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uqq6bdgpqqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1jj7lx7</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Lime fruit</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncz0yz4ukqqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1jj74cg</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>This color gets over shadowed by my skin color. What would you recommend for me?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz3w9u6pgqqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1jj60vf</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>soft gel aura effect🩵1 hour it took! very easy, cute and clean</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3jmacbj7qqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1jj5hhb</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>anyone have tips/products on how to recreate?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppy7gp083qqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1jj5ffc</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>I created these</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj5ffc</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1jj3tog</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Anyone else not satisfied with any type of applicators and end up reliving kindergarten and finger painting?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj3tog</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1jj39qy</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Vintage inspired</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agabxiokmpqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1jj368r</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>I love the seashell pieces so much 🐚🪼🌊⛱️</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj368r</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1jj2ztd</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Grapefruit anyone?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj2ztd</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1jj2qgt</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>my basquiat set</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6igu5qlipqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1jj14to</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>I only used nails sticker</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jj14to</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1jj0ws3</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Made use out of some random nail charms 🍬</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0gp4dw6j5pqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1jizf9g</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Getting streaky lines with gel polish</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jizf9g/getting_streaky_lines_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1jiz3tq</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Guess what my favorite fruit is!😋🍉 freehand on acrylic - 3 hours total</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiz3tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1jiz3fe</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Pink pedi</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiz3fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1jiyb31</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>First time trying a pink and gold combo! What do you think? 💅✨</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hehe48k6noqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1jiwvua</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Bubbles 🫧💙 guess how many hours it took me!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiwvua</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1jiwlgh</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>It's my first time, I did it to myself on both hands</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiwlgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1jitins</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>3 hour soft gel for my cousin 💙</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jitins</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1jit6jl</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Wrong season, but they are a favorite! Fall</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jit6jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1jirhkn</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Loving how these came out!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jirhkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1jiqj1c</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Happy with the outcome 🖤</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jiqj1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1jinlxw</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>cake nails!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jinlxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1jinfoh</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Pretty polka-dots 🔵💅</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c06tnw7g6mqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1jimmj5</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>New pink press on set I did</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fljbwh5tvlqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1jihquz</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Quick Peek - pardon the lint! 😆</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jihquz</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar 26 08:11:27 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_30.xlsx
+++ b/data/collected_data/2025_03_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C513"/>
+  <dimension ref="A1:C703"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9154,6 +9154,3236 @@
         </is>
       </c>
     </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1jk6ktt</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>🐄✨🦓</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4juthk1npzqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1jk6gfl</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Rate my girlfriend's nails, I love them!!!!</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7b8cgmtnzqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1jk5zu1</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>New and leading and failing to remove my stick ons</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f2pf93hhzqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1jk4u6o</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Kiss nail acrylic sets?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jk4u6o/kiss_nail_acrylic_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1jk4neb</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Some growth on my  nail art 🖼️</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk4neb</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1jk4mmv</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>🍸:)</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk4mmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1jk33po</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>nail allergy friends - two words for you : LIGHT ELEGANCE!!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f18tdizwiyqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1jk43d4</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>fairy nails</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk43d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1jk3j6n</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Gel x nails for the first time. Obsesst. Cat eye</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk3j6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1jk3gkw</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Would you get a fill or stretch it one more week?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpobg0xjmyqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1jk30ep</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>🪲 🪲</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xohzgogyhyqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1jk2dts</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Chocolate</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blnh4ejpbyqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1jk26lb</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Broke a nail</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk26lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1jk1t8r</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Practicing my line work</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ivvupwt96yqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1jk1nhi</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>My nails need an urgent change, new color do you recommend?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqujn8ns4yqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1jjzl3z</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>I love the glitter effect.</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90g9gpmnmxqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1jjzg19</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>I can’t tell if these are unsightly or not?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjzg19</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1jjzg4o</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Can I file these down to shorten them? They are gel x nails.</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c4m8t6hlxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1jjz4ii</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Trying press on nails from Claire’s</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjz4ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1jjz8ci</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Running nail salon from bedroom</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjz8ci/running_nail_salon_from_bedroom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1jjz6ho</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Help a newbie- starting self care journey</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjz6ho/help_a_newbie_starting_self_care_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1jjz059</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>👏🏻👏🏻</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uje6mskphxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1jjyy7v</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Simple ,happy with the result</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9btvlhn8hxqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1jjyuob</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My friend is trying</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/levmr6qegxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1jjx5os</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Finally recovering</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjx5os</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1jjx8hr</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>MY NAILS HATE ME</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjx8hr/my_nails_hate_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1jjxv96</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Help please</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuvjj4ve8xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1jjyl8z</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Top coat problem</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjyl8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1jjykqv</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>I like them</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af892s33exqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1jjxyzx</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Don’t sleep on press on nails</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asmeak199xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1jjxvqc</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>New nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be994gfi8xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1jjxezc</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>DIY gel polish attempt #2!</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpq8reyu4xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1jjx8bu</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>my fruit nails in good lighting before the tragic incident!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x0nvm6g3xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1jjx5p7</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Ive finally found my people🥹🥹🥹 fresh set for the New Year 🌼🌱</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa2kfzpv2xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1jjwwps</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Is my pinky nail too long? Something just seems off</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdjyolaz0xqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1jjwruv</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Need some advice!!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ratcmd9xzwqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1jjwohg</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>DIY Press Ons with Gel / Polygel to avoid allergy</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjwohg/diy_press_ons_with_gel_polygel_to_avoid_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1jjwlaf</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Bridal look for short nails?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r1gvxzgywqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1jjwfsj</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Which ones better - red or white?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjwfsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1jjwexp</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Pink rainbow chrome 🩷🌈</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjwexp</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1jjw4ki</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Tried coffin/ballerina for the first time... and loved it! 🤍</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjw4ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1jjvahy</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Purple haze</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upl1pjcpowqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1jjv7vy</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Beetles Builder Gel nails</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjv7vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1jjueaj</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Jocelyn came through with the drip this time 💦🤩</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjueaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1jjtur0</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>What do I get?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjtur0/what_do_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1jju48j</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>be honest please</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vek6ps5gwqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1jjtvyt</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>ISO builder gel (Canada)</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjtvyt/iso_builder_gel_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1jjte39</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Idea VS  results2+surprise</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjte39</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1jjt594</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>They look cute :3</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjt594</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1jjt38e</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>fresh set</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjt38e</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1jjt16s</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Haven't had my nails done in so long but decided to splurge a bit on myself!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wffzq7a8wqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1jjsq4h</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Cute natural nails</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjsq4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1jjrbu3</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>E-file advice</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjrbu3/efile_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1jjrzuq</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>What can I do to make my nails stronger?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a30otqs0wqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1jjrz4x</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Chrome spring nails 🌸</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjrz4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1jjrkg8</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Polish color</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgbn7a4sxvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1jjriaz</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>I painted my nails myself and I think they looked pretty good, didn't they?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjriaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1jjrf8x</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Petals on water</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjrf8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1jjrcxp</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Weak bendy nails</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjrcxp/weak_bendy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1jjraef</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Press ons are my favourite</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0rzl5gpvvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1jjr9xe</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>was feeling this colour coordination today 🩷</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjr9xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1jjr9uq</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>These are horrible lol</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjr9uq</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1jjr5gv</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Cat eye set 🪺✨</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjr5gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1jjqu9q</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Panda pedi</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjqu9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1jjq3tn</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>What do I even do with a nail that's split this badly, this far down?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/qX5p1lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1jjpyue</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>beach themed nail 🌊</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hkr82m8mvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1jjpnm0</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>🍓 Strawberry Nails 🍓</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3g2lb61kvqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1jjpfaf</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Spring Set</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjpfaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1jjp2kf</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>white and silver</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyxl63nqfvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1jjou40</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Help solving top coat dulling problem</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjou40/help_solving_top_coat_dulling_problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1jjot7b</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Got my nails done</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ya6p08vdvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1jjoj84</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Spring vibes ✨️</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjoj84</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1jjo5i0</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Not great at taking pics, but super proud of these nails I did after getting out of the hospital!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oizf3wn59vqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1jjo5yg</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Obsessed with this set 🍎 🐜 🧺</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kmvuiz89vqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1jjnfoa</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Giving my nails a break from builder gel?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjnfoa/giving_my_nails_a_break_from_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1jjmojn</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>I’m not great at taking pics, but I’m super proud of these nails I did to celebrate beating a brutal round of mono!</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rru8cu8yuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1jjnv3v</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Individual colour nails, yay or nay? I love this spring palette</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ki8f1737vqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1jjnewq</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Green nails pt.2!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjnewq</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1jjmqtp</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Hard gel help? I see posts about hard gel being thinner, this doesn’t seem thinner to me.</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjmqtp</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1jjmph7</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Doing my own nails since 2 years</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjmph7</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1jjml4e</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Suggestions</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37vjdmhjxuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1jjmf10</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Keeping nails safe while doing yard work?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjmf10/keeping_nails_safe_while_doing_yard_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1jjm863</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e69px1fwuuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1jjfpnp</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>So I suck at drawing flames but I finally got isolated chrome to work for me (on my husband’s nails)</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wla2ukct5tqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1jjghgu</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>pokemon nails! Togepi inspired 🥚🎀</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjghgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1jjh8mf</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Keeping nails on....</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjh8mf/keeping_nails_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1jjhavn</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Acrylics newbie - questions</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjhavn/acrylics_newbie_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1jjjest</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Nothing fancy</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjjest</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1jjlzso</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Matching my Nintendo DS from 2007 🍑</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8xflbz6tuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1jjlwar</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>New claws</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15qdo9chsuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1jjlusn</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Got my nails dooone</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjlusn</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1jjlswm</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Best shape nail for me?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phnuablsruqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1jjlnrp</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjlnrp/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1jjlfg4</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>My favorite simple nude right now on natural nails. Essie "Sheer Fantasy" 🤍</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjlfg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1jjlc52</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Struggling with nude and light shade nail colors</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjlc52/struggling_with_nude_and_light_shade_nail_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1jjl0gm</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>top coat help</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjl0gm/top_coat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1jjk657</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Press On</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m465cym1fuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1jjjyf8</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>How often do you get your nails done or get infills?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jjjyf8/how_often_do_you_get_your_nails_done_or_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1jjjvhv</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>I found little panda stickers!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjjvhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1jjju7c</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>When you just can’t decide which would look better. Black of white tip</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibzrxxjdcuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1jk5ujv</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Happy with my Collection! 🙂</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk5ujv</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1jk4gb8</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Dazzle Dry - Yoga Mama</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woip3qxmxyqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1jk4b31</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Magnetics that look like the gem tiger's eye</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jk4b31/magnetics_that_look_like_the_gem_tigers_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1jk324c</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Revlon Vixen changed undertone?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jk324c/revlon_vixen_changed_undertone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1jjsji8</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjsji8/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1jk3ss2</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>I always get more compliments on basic colors than all the special polishes I own...</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq6fp958qyqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1jk3eaz</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>When you think you avoided the bubbles…</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4m4lsxvlyqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1jk347l</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Looking for jelly sandwich inspo</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jk347l/looking_for_jelly_sandwich_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1jk2z7g</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Best gel brands on Beyond Polish</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jk2z7g/best_gel_brands_on_beyond_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1jk2o3y</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Mooncat- Forbidden Fruit</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x7v8ljsgeyqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1jk1lr5</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Bendy and Weak Nails</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jk1lr5/bendy_and_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1jk1cnf</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Started messing around with making my own press-ons!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk1cnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1jk1b6w</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Attention Toddler Moms</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezo9e40r1yqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1jk1aoh</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>My first jellies</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4klc5znm1yqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1jk0h6v</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Mooncat’s Siren’s Deceit over Fields of Lavender looks pretty cool!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/afm4gogeuxqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1jk0cux</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Starting off</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk0cux</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1jk0ben</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>"Spring equinox"? How about "cherry blossom season"?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb22gvovsxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1jk028d</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>I dread painting my toes.</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jk028d/i_dread_painting_my_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1jjzeot</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>I'm looking for a black jelly filled with yellow or orange shimmer.</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjzeot</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1jjzein</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>LynBDesigns No One Mourns the Wicked</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjzein</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1jjynv8</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>This pissed me off</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jehus3tsexqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1jjyfbd</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Cat-eye effect in a light color, how does it look ?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06noyfsvcxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1jjy90b</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>fave teal jelly? and fave purple jelly?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnxt32tgbxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1jjxg8h</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Help me refine my indie polish haul!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjxg8h/help_me_refine_my_indie_polish_haul/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1jjx30j</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Mini Cadbury eggs?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjx30j</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1jjx1qv</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Pinking too hard 🧠💅🏻</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjx1qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1jjwqab</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>do I have to file more for almond?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjwqab</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1jjwfys</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Mul Gwishin</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjwfys</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1jjw968</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>LynBDesigns Spring Skittle 🌈</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb75z8uxvwqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1jjw5iz</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Koi Fish Vibes 🫧</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zzp3ysd6vwqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1jjvn7d</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>All pink everything 💕✨</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uaq40perwqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1jjvgyz</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Blind me with sparkles</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.holotaco.com/products/menchie-the-cat</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1jjv3q4</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Swatch of Dolla Dolla Bill Y’all by Cracked</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjv3q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1jju3th</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Tips for growing nail back?!!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z95dym2gwqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1jju37s</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Replacement for Mooncat topcoat?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jju37s/replacement_for_mooncat_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1jju0xk</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Mooncat and Holo Taco comparison</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jju0xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1jjtv6a</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Juicy bright red jelly/sheer recs??</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a5gowt9ewqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1jjtsyx</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Didn’t realize this was sheer</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjtsyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1jjtch4</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>It’s glitter time!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjtch4</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1jjt8qt</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Does anyone know what the Tariff fees are to ship from US to Canada from places like Sassy Sauce?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjt8qt/does_anyone_know_what_the_tariff_fees_are_to_ship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1jjsc83</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Glossy Jordan Almonds</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjsc83</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1jjsawv</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>BKL: is Get Lobstered coming back??</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjsawv/bkl_is_get_lobstered_coming_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1jjs7ks</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>It should be a crime when cameras refuse to fully capture a stunning beauty like this…</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjs7ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1jjqi21</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Dupe Request - Revlon Ocean Breeze</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weg44vg2qvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1jjoztd</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>My signature look, teal to purple ombré</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjoztd</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1jjoz47</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>With a Broken Heart</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjoz47</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1jjoy2g</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Help maintaining glossiness</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjoy2g/help_maintaining_glossiness/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1jjoy0b</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Birthday Suit</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjoy0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1jjousq</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow DaVinci’s Nightie</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjousq</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1jjo5ar</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pokcli849vqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1jjnynd</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>At the end of lessons today, a student came to me and said “I really like the way your nail polish matches your outfit!” That made my day ☺️.</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dtqzs6g8uqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1jjnq6i</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Finally bought House of Hades</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2a6y1vctuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1jjnndg</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Has anyone here tried this subscription?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjnndg/has_anyone_here_tried_this_subscription/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1jjnjdl</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Magnetic “French manicure” setup 🧲</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjnjdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1jjneqt</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Earthy Forest Nails 💕</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjneqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1jjn175</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>immortal jellyfish 🪼</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjn175</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1jjmsr8</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Spring nails 🩵🌼</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih1n6b45zuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1jjmono</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Something is off</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7oe497i9yuqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1jjmkf9</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>A new favourite💜🩵💚</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjmkf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1jjlrgz</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>base/top cost recommendations for peeling polish</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhlluabhruqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1jjl8v9</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Comparison Request: ILNP Lights Out vs Mooncat Bottled Rage</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jjl8v9/comparison_request_ilnp_lights_out_vs_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1jjkyjc</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>wanted to do something for spring, but also wanted to attempt French for the first time</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjkyjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1jjkwcf</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>"Red" Indie Comparison</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjkwcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1jjkqbf</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Am I Everything You Fear?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8lfh14bdjuqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1jjitmw</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Has anyone got polishes from Cosmic Polish (indie Aus brands) would love to seeeee</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x91f6ci3uqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1jjirbf</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>matchy matchy✨</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjirbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1jjio80</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Two colors, two hands? Why not! 💚💙</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjio80</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1jji7ov</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>What brand do you feel is best ‘all around’ ? (ie. color, formula, longevity, etc.)…and why do you feel it’s numero uno?:):)</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jji7ov/what_brand_do_you_feel_is_best_all_around_ie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1jjhxyb</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>⛏️Minecraft⛏️</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjhxyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1jjhu3q</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>My first Lurid mani (of many, heh, oops 🤭)</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjhu3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1jk60dj</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Mermaid Nails | RUMISG</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk60dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1jk0rg9</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>The Gangreen Gang 🦠</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6g17xkywxqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1jjvt3j</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>My sister is a teacher so she will only wear neutrals, but I managed to get her to approve just a little bit of color :)</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjvt3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1jjvrvp</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>mini Easter press ons</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exlijvtbswqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1jjuyig</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Un poco de mi trabajo</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ihu1op9mwqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1jjuqog</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>gold chrome brushed frenchies ✨</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7jti9isokwqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1jjsfgb</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>A little spring DIY design</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjsfgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1jjsbd6</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>My favorite butterfly, I love nail art</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjsbd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1jjrhnx</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>WIP of my next character art</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qxgf2f6xvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1jjr36v</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Sad clown set by moi</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c2kw20auvqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1jjqte8</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Panda pedi</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjqte8</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1jjl18s</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>4-hour soft gel for a friend who is a fan of 🥑💚</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2m4k24euluqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1jjo9s6</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Phasmophobia ghost hunting themed nails 👻💅</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjo9s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1jjn9tf</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Kitty Flower Nails</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ep5fqgn2vqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1jjm1ru</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Honey bees and flowers</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjm1ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1jjlpqn</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>plaid nails! was planning on doing a completely different pattern but didn't have the colors from the inspo pic... but i really like them !</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uupzejf4ruqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1jjkaq9</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>guess which one it is 💚</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjkaq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1jjk5b2</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>What is everyone’s favorite pigment powder(s)?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jjk5b2/what_is_everyones_favorite_pigment_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1jjirxg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Still can’t pin point the aesthetic of this set it too fancy for goblin core but too « dirty nature » for dark academia</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jjirxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1jjenvn</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>I’m going to do new nails, and yes I’m a guy, and I wanted to ask your recommendation on something girly but minimal in art!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7nb2rl3rsqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar 27 08:11:40 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_30.xlsx
+++ b/data/collected_data/2025_03_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C703"/>
+  <dimension ref="A1:C896"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12384,6 +12384,3287 @@
         </is>
       </c>
     </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1jkyvfk</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Green nails for spring💚💅🏻💕</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1302nhpqu6re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1jkytde</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>$55. Love my nail tech</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk5r8tzuu6re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1jky3br</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>New ones 💛😊</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k2433qzk6re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1jkxvh3</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>First time trying nail art 🥹 Still very amateurish, did both the same day my supplies came in.</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkxvh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1jkxp5b</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>love the summer nails!</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psmxpwcsf6re1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1jkxmy2</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Personally, I am a lover of this simple design ✨</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psaagptze6re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1jkxhl2</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpbworazc6re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1jkvz0c</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>What I asked for (thenailen.wordpress.com) vs what I got</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkvz0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1jkwhdv</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Poly gel newbie ❤️</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkwhdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1jkwefh</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Short natural nails forever 💗</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4axapgmkz5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1jkw0vb</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>First time using gel polish!</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c11cjt4bv5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1jkvrmh</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Back with another “protective coating.” First attempt at a marbled design</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkvrmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1jkv776</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>chrome nails to match my chrome nail care brush</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qp8uqz4m5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1jkturq</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>New Nails Monday</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ogxrfdp95re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1jkv3ll</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkv3ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1jkuvyj</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>I QUIT BITING!!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkuvyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1jkur2j</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>how to fix ? please help</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxmyri69i5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1jkukgh</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Spring Pastels French Manicure</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exkeutthg5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1jkuhj2</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>I was encouraged to try this color and the truth is that I loved what they did for me. What do you think??</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by1vs1lpf5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1jkugwn</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Gel X simple ombre</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkugwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1jku2wy</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Btartbox nails</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jku2wy/btartbox_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1jkthl0</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Design ideas?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ewlxc9d65re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1jktgtu</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Robin egg candy themed nails 🪺</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jktgtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1jksvk0</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Birthday nails MHA</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jksvk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1jkslzk</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>WSAF &amp; WSG</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkslzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1jksofi</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Would I be in the wrong to go back to the salon to ask for these dip nails filed down to a more natural/non-bulging size and shape?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jksofi</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1jksq86</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Please help my natural nails</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jksq86</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1jkt7g9</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Out of the blue, gel nails constantly lifting. What gives?!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkt7g9/out_of_the_blue_gel_nails_constantly_lifting_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1jkt4iw</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmqgavv435re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1jksv93</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r65qb7ss05re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1jksu8t</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>DIYed some cat claws!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jksu8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1jkstff</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>The best nail tech &lt;3</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkstff</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1jksopc</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>When you can see yourself and your freshly done mani... ✔️</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s4zsax5z4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1jks9jd</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>HELP.  how to remove</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uqgj9qcv4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1jks96a</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Nails for an interview I had back in February 😍</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl8tqbd9v4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1jks2gg</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Leopard Print &amp; Bows</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2shcztkt4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1jkrhyu</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Strengthener under press ons?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkrhyu/strengthener_under_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1jkrifc</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Got dip powder for the first time and love it✨</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkrifc</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1jkrdth</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>2nd time I did my own nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w83q7sln4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1jkrc0h</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Loveee how my spring nails came out</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkrc0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1jkr9v3</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Sharpened my claws today 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5opf8hom4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1jkr9gl</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>How cute are these!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkr9gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1jkq5zx</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Make a fake nail look 100% Realistic?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkq5zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1jkq0w1</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Cleaning Under Nails</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkq0w1/cleaning_under_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1jkqa91</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au14cemfe4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1jkq42a</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>What do you think? (Before &amp; after)</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkq42a</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1jkpx9y</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>New lil beans</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkpx9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1jkpkdd</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>My new simple black-pierced set 👽</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkpkdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1jkpevw</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>First time painting my nails, idk if the colour is good for my skin tone or not</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkpevw</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1jkp4kf</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Love 💚</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkp4kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1jkofnd</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Inspired by a sticker</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkofnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1jkotet</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Cake nails in honour of cake day on Friday 💖 I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgtk1p0z24re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1jkorb6</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Are my nails too short (or otherwise ill-suited) for a structured mani?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msj7wzfi24re1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1jkolqm</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Gel x - love length &amp; shape, not into the color 😩😩 is it easy to change it!!!??</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkolqm/gel_x_love_length_shape_not_into_the_color_is_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1jkokv6</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>It made me very nostalgic, these are some of the first nails I did :')</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rtqr1ro04re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1jkoi9m</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>ISO!! Nail artist located in WA!!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkoi9m/iso_nail_artist_located_in_wa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1jkohkn</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>i want to be a nail tech, this is my second work. do I show promise? any advices?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkohkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1jkognr</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Pink and blue</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djrmj8m504re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1jkoe96</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkoe96</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1jkobxq</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>❤️ LOVE</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwactn54z3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1jkoanj</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Comic Book -Spring set</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkoanj</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1jkntim</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>I got pink glitter dip and wish I hadn't</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkntim</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1jknfhg</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>my nails come off so easily.</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jknfhg/my_nails_come_off_so_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1jkn8o8</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I love my manicurist, she's just magic</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8m9u9nsq3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1jkmsy5</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>REPO inspired nails!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkmsy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1jkmlvy</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>New Spring Nails 🐣</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkmlvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1jkmh28</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Beetle inspired nails</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkmh28</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1jkmg4e</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Stickers</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkmg4e/stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1jkmedj</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My first time trying builder gel, how did I do?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkmedj</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1jkm1gs</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>My First Skittle</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkm1gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1jklpqb</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Great Gatsby Vibes</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k84qhg6cf3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1jklebp</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Need help deciding which polish suits me the best, I'm more of a natural nails girl and it's been a while since I colored my nails.</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svu0mqu2d3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1jklhzf</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>peach set 💖</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jklhzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1jkl2i4</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Got way too impatient and ripped off my nail polish- will my nails heal or are they stuck like this?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkl2i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1jkkkps</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Loving my deep red French with chrome!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkkkps</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1jkkhdj</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Valentino Rossi inspired Nails for MotoGP this weekend</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep5ok0of63re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1jkkhea</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>I love how my nails match me, my manicurist showed off too much🖤🖤🖤</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwffcsbf63re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1jkk2ip</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Ring of fire solution during grow out?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qzhikk723re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1jkkf4a</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for this shade of 90s Wet and Wild nail polish</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl8ntzaz53re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1jkk5kf</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Nails for prom that would go with my dress?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqm1db7w33re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1jkjs9e</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>love them</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkjs9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1jkild3</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Nail glue vs sticky tabs?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jkild3/nail_glue_vs_sticky_tabs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1jki8nm</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Mix &amp; match nail art has been sparking joy lately! 💫</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jki8nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1jki5r2</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>First time getting Gel X. I’m in love!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udq20mogp2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1jkhrr4</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>What I got vs Inspo from Pinterest by @kmnloretta</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkhrr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1jkhp2o</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>nails from a few months ago!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a214pox4m2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1jkhjjp</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Love these</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zmus0b0l2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1jkhg44</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>new set☀️</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cn975mvbk2re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1jkh5gx</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>First time doing my own nails with gel and gelpolish! What do you think?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd714mx8i2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1jkgrzw</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Perfectly simple 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdl70o3jf2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1jkgnje</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Spring colors</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkgnje</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1jkgd9e</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Purple flames to match my energy</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqaj246lc2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1jkg6mq</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>How do I fix this surface mistake on salon gels?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5930cyo7b2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1jkd0hb</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Spring Showers in Cashmere Blue</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkd0hb</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1jkffc1</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Cherry blossom spring nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkffc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1jkfch6</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Looking for this gradient as a polish 💅</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pnpgf0052re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1jke0t2</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Meta Post - Bride / Bride to Be Nails</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jke0t2/meta_post_bride_bride_to_be_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1jk74od</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>How do we feel about this thickness of french tips??</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9o5fo8ixzqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1jkc0mn</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I can’t tell if I killed these or they killed me</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkc0mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1jkf59w</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Obsessed with this style!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mfzrvzl32re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1jkxo2e</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Cracked Polish - Cupid Missed Swatch Request</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkxo2e/cracked_polish_cupid_missed_swatch_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1jkfqp3</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Another Flower Child post</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w0jhdad52re1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1jkjda7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Cuticula Fairest of Them All – Minty Flakie Magic! ✨</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkjda7</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1jkqwvu</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Butter London ‘Crumpet’ dupe.</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlpj2y2lj4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1jkrsnn</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>does this nail shape suit me?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fessoqn7r4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1jkv5ww</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>What polishes are so good they save you money?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkv5ww/what_polishes_are_so_good_they_save_you_money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1jkv3q3</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Does anyone ever put a clear coat between or under flakie layers to give them more dimension?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikoq45mql5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1jkv2gg</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Black to red flakes?? Have you seen this before? Whats with so many releases on the 28th?!</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkv2gg/black_to_red_flakes_have_you_seen_this_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1jkuyd4</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>ISO stamping plates construction/archaeology themed</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkuyd4/iso_stamping_plates_constructionarchaeology_themed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1jkuk1v</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Cephalopod magic up</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkuk1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1jku0a1</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Top/base recs</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4as4t66b5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1jkty8u</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Been practicing doing my own nails, was happy with how these came out</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh45amema5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1jkti7u</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>How many polishes do you think the average non-polish obsessed person has?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkti7u/how_many_polishes_do_you_think_the_average/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1jksse6</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>A little beginner nail art for your viewing pleasure.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6xqbij205re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1jksrpw</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Flakie Madness</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jksrpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1jksor0</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>I feel like a fairy 🧚</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xafx78x5z4re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1jksi8k</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>pool nail perfection✨☁️</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iztapgiix4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1jks8zv</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Nail Art progress</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jks8zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1jks83s</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Obsessed with this polish</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jks83s</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1jks10k</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>How do I layer a nail polish with 24h dry time?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jks10k/how_do_i_layer_a_nail_polish_with_24h_dry_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1jkrojk</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>I swear I'm wearing a "neutral" polish</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkrojk</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1jkrnuk</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Matched my nails to academic regalia 🧑‍🎓</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14xvyrb1q4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1jkri66</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>I'm search of the perfect Velvet cateye</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkri66</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1jkrhsp</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>medusa ✨️</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkrhsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1jkq84n</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Been feeling nostalgic for Y2K lately.</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzq3iftzd4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1jkpz8a</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Rainbow charm moment - obsessed!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkpz8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1jkptqn</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>OPI teenage dream dupe - Moonshine Mani</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkptqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1jkpgnu</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Arc magnet for lacquer cateye win 😻</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8hfw14fz74re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1jkpglo</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Can you use reusables for nail polish removal?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkpglo/can_you_use_reusables_for_nail_polish_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1jkoq2v</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Love this idea!</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8sez5l824re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1jkops5</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Love How These Shades Coordinate!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkops5</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1jkon2m</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Stamping is so fun!</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkon2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1jkodcy</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>I get the hype of mermaid bait!!!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8kuit7gz3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1jkobw2</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>A little messy but still pretty</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkobw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1jknvxu</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>This is THE most perfect glittery gold ever</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jknvxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1jknv5s</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Toddler's choice mani</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atotn9rjv3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1jknsgv</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Magic Magnetics ✨🧲</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jknsgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1jkme65</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Mishipeshu-The Great Lynx (LynB)</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acytequek3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1jkma0t</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>BKL - Lemon</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jll2c8ihj3re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1jkm1sl</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>New ILNP collection coming..guesses?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmmaatxsh3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1jkluoq</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Anyone know why this happens or what this is?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pp7jrpacg3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1jkltnk</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Do I cut them short?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkltnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1jklncq</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Was unprepared for how much I love this color</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfprcabve3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1jkkscz</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>The color blue has me in a chokehold</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkkscz</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1jkjw6w</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>ISO Iridescent toppers</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkjw6w/iso_iridescent_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1jkj7mq</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Here comes the party poop</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkj7mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1jkj2gs</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Finertips still extremely dry 2 days after soaking off gel polish with acetone?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkj2gs/finertips_still_extremely_dry_2_days_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1jkibtg</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Mismatched nail art has been sparking joy for me lately :)</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkibtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1jkh7i3</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>this was an absolute fight for my life…</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40kqh4rmi2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1jkh1iu</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>When your nails match your shirt 💚👀🧌🦇😁</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jf7hu46h2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1jkgx24</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>First Death Valley purchase- pardon the stumps.</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmln76hig2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1jkgv9s</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>LA Colors - Wanderer</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkgv9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1jkgm1s</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Sparkles!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k51u35dde2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1jkgekd</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Beginner AF nail art</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkgekd</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1jkgcgk</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>ILNP Lily! 💜</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkgcgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1jkgc5y</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Color block nails, prep tips?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkgc5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1jkgbn4</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>KBShimmer Favorites</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkgbn4/kbshimmer_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1jkg62b</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Sunset Nails 🌄 (Norpsilocin)</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkg62b</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1jkg20k</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Hopped on the cabochon train</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkg20k</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1jkfey8</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>First Lurid Haul with 2 Prototypes</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkfey8</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1jkfdse</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Moonwake</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkfdse</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1jkez1n</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>How bad are my cuticles?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7jqpicb22re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1jkeu4m</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Duped myself twice with this shade. Hopefully the comparison can at least be helpful for you guys!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n1ss46j912re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1jkegol</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>How can I remove dye stains from press on nails?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkegol/how_can_i_remove_dye_stains_from_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1jkdxo9</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Mooncats Lovebomb 💣💜🩷</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkdxo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1jkdwkn</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>I'm legit in love with gray nail polish</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkdwkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1jkd9cg</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Holo Glitters?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqbag9v7p1re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1jkd4qu</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Just my small globby flowers and crusty cuticles</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkd4qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1jkbfr2</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Why does my thermal do that?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi258kd5a1re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1jkbb3x</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Spring flowers!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4rvbipd81re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1jkb6fp</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Nail shape is everything!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jkb6fp/nail_shape_is_everything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1jkb3oh</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Hello spring 🌸🌺🌻🪻</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxxe9i1b71re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1jk9k16</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Mooncat - Maelstrom</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk9k16</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1jk8wmw</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Spring Palette🌸🦋🩵🌿</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk8wmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1jk7f9i</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>From the a-england sale</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk7f9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1jk6w63</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Little haul from Japan</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk6w63</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1jkysob</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I hate being my own nail tech sometimes</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkysob</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1jkwlpk</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Blushing Stars 💫 Soft pink with a cosmic twist! What do you think?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqajlppv16re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1jkwa38</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Clowning around at work today 💅🤡</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76i7xo28y5re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1jktdjv</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Floral nail art 🌻🌺🪻</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1079p0c55re1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1jkssd4</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Day of taking pics to nails before a new design 🩷</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69kl4sc305re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1jksd2e</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Bubbles in my cat eye polish 😭😭</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jksd2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1jks9ce</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Prom nails?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jks9ce/prom_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1jkptz2</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I’ve been feeling nostalgic for Y2K lately.</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usy1wx1wa4re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1jkofzk</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Pink and blue</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o5yc1g004re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1jkm3mi</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>First aura nail attempt</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r3y2me6i3re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1jkixzm</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Will it be okay for a bank worker?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkixzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1jki3ep</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>First time doing my own nails with gel + gelpolish. What do you think?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bqsbf2zo2re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1jkfu4q</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>I wanted to recreate a set I saw by a YouTuber, Glamify Babe.</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkfu4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1jkdo7w</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Lichen and moss nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkdo7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1jkcphn</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>one of my clients asked me for hearts only to see if she would have luck finding the love of her life 😂😂♥️</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a199yktvk1re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1jkcawn</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Spring is in the air, new color changing design🐝</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jkcawn</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1jk8uc9</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>whimsigoth inspired nails ! shockingly proud of these as someone with no artistic ability.</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jk8uc9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar 28 08:11:52 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_30.xlsx
+++ b/data/collected_data/2025_03_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C896"/>
+  <dimension ref="A1:C1085"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15665,6 +15665,3219 @@
         </is>
       </c>
     </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1jlq44n</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Barbie press ons 🩷</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlq44n</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1jlpz97</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Birthday nails: Purple-Pink-Orange Aura with mermaid chrome, 5 XL Stiletto Gel-X Nails</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlpz97</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1jlptm8</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Last two sets I did!</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlptm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1jlp0wu</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Is this good work? I’m happy with them, but I know nothing about nail art (50€ in Germany)</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlp0wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1jlow21</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>my first ever acrylic set!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jyu0me5ldre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1jlo4uw</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Obsesionada con estas nuevas uñas.</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/175d79hnbdre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1jlnm8e</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Pretty in pink 🩷</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8henkrm5dre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1jlnm5x</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Maybe "simple" it's enough sometimes</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a5gwp0m5dre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1jlnhb7</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>rings of fire?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgwrlg054dre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1jlnetq</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>question re: gel nails</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6ol6oxb3dre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1jln2fm</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Wedding nails on my honeymoon 👰</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jln2fm</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1jlmptz</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>O que que eu preciso fazer para deixar minhas unhas fortes?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7d4cuorvcre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1jlmlsm</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>🌼🌷🐝🐞</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlmlsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1jlmaif</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Jus messing around, 😁 many layers..</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlmaif</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1jllref</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>The reason for hands hurting this week</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jllref</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1jlle69</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>It’s cherry blossom season! 🌸</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00sy6q2vicre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1jllcbv</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Opinions on DIY method</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jllcbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1jll5gv</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Attempting extensions for the first time!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jll5gv/attempting_extensions_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1jlko8c</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>a little grown out bc my nails grow so fast but new here so wanted to show 😫</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0o69t45ccre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1jlkkxs</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>My manicurist continues with her ideas and I show you one of her works today.</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yrv4e5bbcre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1jlkae6</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Nails for my Tattoo Artist</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84gctoum8cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1jlk65t</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz829cjl7cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1jlk4yz</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>I really hate how sloppy the nail art is for the price I paid.</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlk4yz</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1jlk3t2</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>I’ve never gone pointy before.  How do they look?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlk3t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1jlk2k7</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>First time using builder gel over gel x tips. CCW</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlk2k7</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1jljut1</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>beginner attempt at stain glass</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t22fb6q4cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1jlju6j</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Hey everyone. I do polygel nails. I want to start teaching online but don’t know how or where to start.</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlju6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1jljgiq</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Melody Susie lamp safe?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcthn0061cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1jlj2fu</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Spring time nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1m1u2iypxbre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1jlit11</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>tried an american manicure with a spin for the first time and i’m really liking it :))</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovhn9nmevbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1jli6fg</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Red Nails🍒</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jli6fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1jli3vk</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>A wee bit obsessed with Sunflower Nails 🌻💛</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3movsavbpbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1jli12e</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Funky &amp; fun spring set 💚🌿✨</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jli12e</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1jlggai</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Not sure what to do about horrible manicure experience.</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c51qh9t0cbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1jlfujl</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Leave em matte or go glossy?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlfujl</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1jlfqse</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Fake nails not coming off</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlfqse/fake_nails_not_coming_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1jlhwp6</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Tried 3D gel for the first time and here’s my attempt at blueberries</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nmyuy0onbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1jlhufr</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>PLEASE help me find this combo! OP Insta Handle is @__takamuu__</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DGlCMEmBs1g/?igsh=MTg1ZzFraGJ2ZGI5ZQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1jlhs3i</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I love cat eye so much</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xavhhfukmbre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1jlhrs3</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Besr DIY nails?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlhrs3/besr_diy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1jlhk8e</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>First attempt at cat eye</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g9tojqprkbre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1jlhcxa</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Why do I hate them? Design feedback please!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dngxa544jbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1jlhaid</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>I know I’m late but wanted to share the nails I did on myself for Valentine’s Day💖</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kecnyscjibre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1jlh6eo</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>First time trying out blue sparkle cat eye. 👁️</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6c9nosnhbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1jlh1th</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>3 Hours Later 😭😂</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upfip44ngbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1jlgs4i</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>My mom's nails</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlgs4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1jlgplt</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Haven't gotten my nails done in forever</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlgplt</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1jlgfit</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Made today by me on me</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qowenn9tbbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1jlgd5q</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Which nail shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wry1elpbbbre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1jlg61y</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Should I try almond shape?</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlg61y</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1jlg20f</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Are these bad</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdk0ljsx8bre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1jlg1ol</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Chip :(</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izs9p59v8bre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1jlfztt</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Birthday nails 💎</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsrg364h8bre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1jlfwsw</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>I love this season! My favorite colors together !</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gman0vut7bre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1jlfpig</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>🍯🐝</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlfpig</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1jlfj48</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Question about cost?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlfj48</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1jlf25j</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>I’ve never had nails this bright before, I think they’re so cool</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlf25j</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1jleis6</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Finally got my red cateye</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r66l7rufxare1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1jleid4</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Obsessed with this new spring set 🍃💐</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg3kl32dxare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1jld0bk</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>what do i do after acrylics?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jld0bk/what_do_i_do_after_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1jle1e0</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Got gelX nails, didn’t like the gel polish I got on them. What can I do?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff6ga4bztare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1jldu81</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>there’s something so nostalgic about a french manicure with black 🖤</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qqjbuclsare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1jldmc0</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Got these done yesterday. I'm in pain, but they're so pretty.</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jldmc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1jlb2tw</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Full coverage press one</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlb2tw/full_coverage_press_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1jld0sp</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Help me find my dream gel polish please !!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jld0sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1jld2i1</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Gel allergy?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jld2i1/gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1jldb0w</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Soft floral pedi</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8ygqzotoare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1jld9rx</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Squavoal or Almond?😸</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stjlm3uhoare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1jlcl9o</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>A demure little press-on set</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h4nq14qpjare1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1jlcilw</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts 358/2 Box Art Roxas as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlcilw</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1jlcdkr</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Tipping?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlcdkr/tipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1jlc9xi</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Tried French tip nail art for the first time first time</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlc9xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1jlc4uu</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Acrylic question</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxc4sffgfare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1jlc17j</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Tried press on’s</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/habmoev3dare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1jlb8t4</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Are these crap or should I go back to press ons?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlb8t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1jlb8f6</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Are these crap or should I go back to press ons?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlb8f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1jlay2w</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Squoval?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlay2w/squoval/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1jlaxuz</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>How do i find out the proper sizing of my full cover tips (from a newbie press on business owner)</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlaxuz/how_do_i_find_out_the_proper_sizing_of_my_full/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1jlabhy</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>This design was suggested to me by my manicurist, I love the color, the details, everything⚜️🌸.</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yumjpbu5v9re1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1jla1xd</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>I’m getting my nails done for grad pics.</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jla1xd/im_getting_my_nails_done_for_grad_pics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1jl9x6j</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>I hate what I done</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auq9qor6s9re1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1jl9sa6</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Nail color to match this dress?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jl9sa6/nail_color_to_match_this_dress/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1jl2ha8</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Worried about my cuticle after last weeks appointment. Please read</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl2ha8</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1jl9bfx</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Favorite/Best press on nails?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jl9bfx/favoritebest_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1jl93xj</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Anyone else on the Acrylic struggle bus? 🥲</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx146rq6m9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1jl8vup</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Spring vibes🌸</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz21ynakk9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1jl8rzp</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>nails i have done so far in the past few months</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl8rzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1jl8lho</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Snake birthday nails</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl8lho</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1jl8jcq</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>My nails right now &gt;&gt; feeling so cute with this set :3</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yga76q81i9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1jl8gzc</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>help 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jl8gzc/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1jl8ce2</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>And THIS is why I do my nails at home. This is just two short weeks of growth.</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymc9gh5lg9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1jl89iv</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Salon only put one thin layer of clear gel top coat</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jl89iv/salon_only_put_one_thin_layer_of_clear_gel_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1jl4okh</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>First attempt at DIY press ons</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjsbusvno8re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1jl2jt7</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Jade/geode inspired nails! 😍</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl2jt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1jl21t6</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Help 😭 my nail designs keep chipping off 🥲 i literally did these like 4 days ago and theyre already chipping off- this has never happened to me before!</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl21t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1jl1jd5</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Claude Monet inspired nails I’ve done 🩵</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl1jd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1jl7px6</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>My Nails making a podcast</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vgy177ptb9re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1jl7936</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Strawberry Picnic 🍓🧺</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl7936</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1jl763i</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Slanted nails</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl763i</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1jl73p2</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>BIAB set on my own nails for practice, please let me know your honest thoughts</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhkpdzkb79re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1jlpkeg</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>I have NEVER been this excited for a collection before?!??</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlpkeg/i_have_never_been_this_excited_for_a_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1jlp1sd</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Does anyone else miss MissHollyBerries YouTube videos? 😩</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlp1sd/does_anyone_else_miss_misshollyberries_youtube/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1jlo9zk</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>mother of pearl lacquer</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/22cvhbydddre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1jlnpbv</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Anyone know what gel this is?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlnpbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1jlmu8j</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Battle of the Blues 💠</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/egcbgv90xcre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1jllwiy</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>TIL the Smithsonian has a nail art exhibit</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.si.edu/stories/museum-inspired-manicures</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1jllmvd</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>ILNP price increase on Amazon?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66sd2725lcre1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1jlljk4</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Just here to drop some Big Reef Energy.</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9oirb9kpjcre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1jlkwvt</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Selena Gomez’s Hot Ones Nails!</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faq650scecre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1jlkuut</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>How much product do I need to remove before "new" mani</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlkuut/how_much_product_do_i_need_to_remove_before_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1jlk7i9</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Can water-based polish be revived?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlk7i9/can_waterbased_polish_be_revived/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1jlk7er</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Beware of fake Mooncat ads!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bsv7z5sw7cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1jlk0y7</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Baroness X Octo-Alien</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlk0y7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1jljmto</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>I feel like this is the perfect vampiress red</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwo3v3gb2cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1jljiec</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Dont know how I feel about the accent....</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jljiec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1jlisv0</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Nail drill thing = my worst nightmare</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlisv0/nail_drill_thing_my_worst_nightmare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1jlidj4</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>My Pet What?! ft. obligatory pet</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlidj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1jli8u9</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Recommendations for creme shades</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jli8u9/recommendations_for_creme_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1jlhy08</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Caught this beauty under some sunlight and had to share!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7w1dzjrynbre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1jlhbym</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clehzthwibre1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1jlh61t</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>To gel or not to gel?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlh61t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1jlgauo</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>The Base and the Coat (round 6)</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlgauo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1jlg791</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>This is all one polish</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlg791</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1jlfdq0</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Couldn’t decide which pairing I liked better, so I did both 🤷🏼‍♂️</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlfdq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1jlfbkn</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>sprang thangs</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0fo4x5c3bre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1jleth4</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>flakie season 🐉</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jleth4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1jlekzs</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Enchanted to Meet You</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlekzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1jleja5</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>does anyone else find a ray of sunshine and do this? BAM! BAM!</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ji2wyi6jxare1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1jle3ch</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Orly 5$ polishes!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jle3ch/orly_5_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1jle1v6</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Acrylics question</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jle1v6/acrylics_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1jle044</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Never Tide Down</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvs00rlptare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1jldr16</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Got this beautiful set today!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2tyi1eyrare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1jldp8t</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>BKL Betelgeuse💛💚</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jldp8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1jldo7g</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Suppliers</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jldo7g/sassy_sauce_suppliers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1jldnrc</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>BKL 💙Enemies to Lovers💜</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w174y1earare1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1jldcpq</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Favorite purple glitter combo! I call this Serpent Dust 🐍💜</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jldcpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1jld3ao</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>First time I was sad to remove nail polish for my next set 🥲</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jld3ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1jld36w</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>What are your favorite nail polish brands and why?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jld36w/what_are_your_favorite_nail_polish_brands_and_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1jlcxxl</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Three vs two coats Cock a doodle doom</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gxcsi99zlare1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1jlcebx</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>What do y'all use to thin your gloopy top coats?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlcebx/what_do_yall_use_to_thin_your_gloopy_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1jlc3t2</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Cuticula Has AMAAAAZING Customer Service, just wanted to Shout Out</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlc3t2/cuticula_has_amaaaazing_customer_service_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1jlbz9a</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>my regular polish takes forever to dry, any hacks?😢😢I miss gel polish but I had to stop because it took too long to remove it</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlbz9a/my_regular_polish_takes_forever_to_dry_any_hacksi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1jlbk2a</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>How are we achieving this look??</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhx8gzm74are1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1jlaerd</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Thermals might be my new favorite🩷💙</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlaerd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1jl9yai</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Never would’ve thought that I’d become a green nail polish girlie 💚</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl9yai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1jl9hrb</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Soooo glowy! ✨</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2e7it7zo9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1jl9gs5</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Opal IS a neutral!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl9gs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1jl91ow</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Mooncat Plankton</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl91ow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1jl887a</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>🩷💛Pastel Leopard💜🩵</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl887a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1jl859g</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Shifty Magic</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl859g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1jl7ykn</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Spring trim!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl7ykn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1jl7wfe</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Tips for cleaning acrylates off tools?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jl7wfe/tips_for_cleaning_acrylates_off_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1jl7tfp</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>First time with reflective glitter!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqpat0mnc9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1jl7od0</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Moody Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ru0adrbep1re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1jl7jxi</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Deserving of the hype</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yocswxnoa9re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1jl77ot</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Help me solve this nail shape conundrum</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl77ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1jl76o7</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Is nail polish as paint dangerous?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jl76o7/is_nail_polish_as_paint_dangerous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1jl75li</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>We have deep sea at home…</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl75li</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1jl745b</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Needed a mood boost</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9uvcv8779re1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1jl6s3o</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>The blessed combo, on homemade extensions.</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl6s3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1jl6rxn</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Disco Poltergeist</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl6rxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1jl6i2k</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Ion the Prize 🧲</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l2fgzhjp29re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1jl64rt</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Why can’t I fall in love with this polish?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk3cnfnwz8re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1jl5l3g</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Cabochon Collection Swatch</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl5l3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1jl5bzr</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>ILNP Lightwave 🫧</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x70u4n0tt8re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1jl565r</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Bendy Nail Help!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl565r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1jl4fdd</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Base Coat Battle: Round Six</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl4fdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1jl3wgm</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>House of Hades really is that Bitch</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl3wgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1jl3mav</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>I was going for a vampy look 🌙🥀</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j34m7kzdf8re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1jl3m2x</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Spring Pearls</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl3m2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1jl3bpk</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Feeling like a disco ball with Tectonic Shift!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jnhm9ijc8re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1jl2liv</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>i know a blurple hate to see me coming</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl2liv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1jl2jc0</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Forest fairy themed nails using a polish with a very unfairy like name</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zsgqsraa58re1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1jl1fkk</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Princesses rule!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl1fkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1jl0s6p</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Cirque purple jellies</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jl0s6p/cirque_purple_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1jl0ov0</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>I asked my nail tech to be creative and k! nky</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ppsd5osk7re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1jlmp6s</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Spring flowers</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u0fcxxkvcre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1jlmnmu</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Juicy jellies</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlmnmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1jllxuj</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>What else can I add?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wheota80ocre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1jlle7n</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Should I redo the same spring nails?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odwaswcvicre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1jlkspm</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>UPDATE: 3D sculpture gel not fully curing</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlkspm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1jljtma</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Hard gel with cat eye, I’m obsessed with this Chinese nail art aesthetic</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp58j4sf4cre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1jleas0</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>First Easter mani</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jleas0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1jlda1b</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Soft floral pedi</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7u4e4gmoare1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1jlcl9h</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts 358/2 Box Art Roxas as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlcl9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1jl9hzt</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Self nail</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl9hzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1jl67fb</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Para las amantes del color azul 💙💙😊</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxlle7gh09re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1jl21yq</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Pink girly nails 💓</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9jsuxoh08re1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1jl1ljt</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>3 hour soft gel for a client who became a friend 💖</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jl1ljt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar 29 08:10:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_30.xlsx
+++ b/data/collected_data/2025_03_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1085"/>
+  <dimension ref="A1:C1278"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18878,6 +18878,3287 @@
         </is>
       </c>
     </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1jmgf1w</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Well, fck.</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu99tw0brkre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1jmgadr</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Builder gel directly onto natural nails?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmgadr/builder_gel_directly_onto_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1jmfyed</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Trying something different for spring</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28yrej68lkre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1jmfvwx</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Second time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgjexz9ckkre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1jmf28x</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Love my spring set 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l31y89sdakre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1jmeune</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>(OC) Sometimes, I like to do themes for my nails based off the week I've had. This week, we lost a family member and so I dedicated my nails to the unsung hero of this time: ✨️Ibuprofen✨️</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmeune</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1jmec0y</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Tried a new and they did not disappoint</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pudtae22kre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1jmdowd</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>First time with getting acrylic, so odd having longish nails.</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1lnj9b5vjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1jmdumb</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Purple?~</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmdumb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1jmdvp7</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Some of my work (self taught amateur)!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmdvp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1jmdbdl</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>tales of a reformed nail biter 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmdbdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1jmcub2</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>What fits my hand better? Almond or coffin?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmcub2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1jmcjjm</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>A moment for the nails.</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g8b87dtjjre1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1jmc0em</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Gel allergy</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmc0em/gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1jmc9n4</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Sister date - what do you think?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uird2wu3hjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1jmc0rc</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Spring has sprung 🌸🌿</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmc0rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1jmbs68</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Asked for Spring themed and the tech delivers!! (They’re one week old 😅)</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkx2r74kcjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1jmbonj</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Is this a gree?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8c6ig1nbjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1jmblrl</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Some of the Nail Art I’ve done✨</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmblrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1jmbk43</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Mani Day 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfj90svgajre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1jmbdeu</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Cinderella chrome with glitter 💙✨</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry6p39gq8jre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1jmb1af</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Fresh vs 5+ weeks growth 💅</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmb1af</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1jmax66</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Please critique</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmax66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1jmaq6e</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Spring nails 😍</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmaq6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1jmanmw</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>What nail extensions would fit what I'm wanting?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmanmw/what_nail_extensions_would_fit_what_im_wanting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1jmakil</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>What should I do next for my nails?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv31krte1jre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1jmai9h</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Which shape looks the best please? ☺️</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmai9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1jmadvd</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Duck nail press ons</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmadvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1jma99w</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>These are my natural nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jma99w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1jma50i</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>I only ever had acrylics done once, this was the result. Is it a bad tech or are these results good? I want to get acrylics again but I don't want them to look so bad next time. My thumb is the worst but I don't have any good pics of it</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jma50i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1jm9xgz</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Gender reveal nails</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm9xgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1jm9w6o</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Cute and Simple🧡</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1g3ebiibvire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1jm9k0m</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>3D nail art</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm9k0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1jm5n83</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>How do you pick your color?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jm5n83/how_do_you_pick_your_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1jm5sae</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Hunger games inspired mani, just finished SOTR and I have a lot of emotions so this is my coping mechanism 😭</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm5sae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1jm8lu4</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>How my cheap ass made nail holders</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm8lu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1jm8ib5</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>My new spring set!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kprbdnejire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1jm84sr</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>best hand moisturizer for a psoriasis girly?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jm84sr/best_hand_moisturizer_for_a_psoriasis_girly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1jm804e</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Funky frenchies 🌊🤎</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm804e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1jm6x89</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Tips for opening OPI nail lacquer bottle?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jm6x89/tips_for_opening_opi_nail_lacquer_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1jm7p11</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>White polish keeps seperating</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sj1pyhrcire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1jm7nri</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Need a recommendation</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jm7nri/need_a_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1jm78hf</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>New nails for sakura season; they're gifted 💅🌸🌸🌸</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn4cbyv09ire1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1jm75xy</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Love these!!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omluqemh8ire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1jm6v5o</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>🍑</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdat4h556ire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1jm6dxe</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Rose chrome v2 ft. henna</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko8tddid2ire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1jm5xgd</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>First time doing fake nails on myself</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf7qja2oyhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1jm4na4</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Question about soaking off acrylic with cut cuticles</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jm4na4/question_about_soaking_off_acrylic_with_cut/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1jm53x2</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Anyone with a gel allergy (or without) used Artificial in a Flash??</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ts8imx2eshre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1jm5crn</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Digital inventory</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm5crn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1jm5bz0</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Digital inventory?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm5bz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1jm564q</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Limoncello from Le Mini Macaron with their short coffin gel extensions 💛🍋</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm564q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1jm53ov</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Blue for spring?</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry1y1z35shre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1jm52o7</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I did some little watermelons this time 🍉</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxqcd4z4shre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1jm51a7</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Hard gel manicure</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5bs19burhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1jm4zv4</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Simple mint green nails 😊</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4zv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1jm4wy9</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>New nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijk0xa1xqhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1jm4vtq</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Mermaider polygel set</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4vtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1jm4qhr</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Stellar Evolution ✨️</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4qhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1jm4i21</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>How to keep geometric designs consistent?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4i21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1jm448v</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>why did my nail polish shrivel?</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm448v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1jm3owb</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Snowy Spring Day 🌼</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm3owb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1jm3ndq</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Did my own Gel-X birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm3ndq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1jm3mqd</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>my tech never leaves me disappointed</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z562ag33hhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1jm3k6d</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Glamnetic Santorini</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm3k6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1jm3co4</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>I went bright for spring</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zj1ms8xxehre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1jm3aa8</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Do we talk about press-ons here, or are they frowned upon in this sub?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm3aa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1jm2sm1</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Vacation Nails!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm2sm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1jm36f4</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Efec ojo de gato 🖤</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb1sxyrmdhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1jm3239</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>First time playing with solid gel</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/44dxva7qchre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1jm2y2s</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Yes or no?💅💅</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yesionlvbhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1jm2ftx</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cmiklj38hre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1jm289k</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>It was all good until …</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm289k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1jm1quc</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Bohemian spring pedi</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm1quc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1jm1nil</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Help with trying to grow/strengthen my nails?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm1nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1jm1i61</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Razzle dazzle 🍒💋✨</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm1i61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1jm1h0m</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Milky lavender &lt;3</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm1h0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1jm1exp</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Giving up on salons: Six dollar press on going 2 weeks strong</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apcerlfc0hre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1jm1bq6</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>went to someone in home and won’t go back!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hviacieozgre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1jm1ac4</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I’ve never had such an amazing set!!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcyhbkyfzgre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1jm1251</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Simple &amp; cute</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvdefpfoxgre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1jm0u8w</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Nude 🤎🤍</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm0u8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1jm0tyj</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>April set 💙🩵🤍</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm0tyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1jm0mg5</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>New to Nail Art</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81za5ohgugre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1jlmgjp</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>new to gel x</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlmgjp/new_to_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1jm0fz1</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Easter Nails 🐰</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm0fz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1jlmq7w</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Looking for Press ons or recs</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlmq7w/looking_for_press_ons_or_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1jlt2jj</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>White polish going discoloured?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlt2jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1jlzvdq</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Workplace appropriate gothic nails 💜🖤🦇</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uyba8q8uogre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1jlza48</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Cute Spring Ombré French 🍧🌸</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlza48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1jlzggd</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Is there anything i can do to fix this?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdljgyetlgre1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1jlyzvn</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Does anyone know what might be going on with my nails?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlyzvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1jlyk7y</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>🦄 chrome</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxjtiu2segre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1jlyha7</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Sparkly limes 🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15lrb0b8egre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1jlyg8m</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Work moisturization without the mess</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/32dy4qmhdgre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1jlydlc</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Quick set of press-ons</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k47ie0gdgre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1jljx52</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Tingly palms</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jljx52/tingly_palms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1jlkvub</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>OUCH! COLD ACRYLICS!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlkvub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1jly030</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>My 4th attempt at acrylic.</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jly030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1jlszqy</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Don’t pay for pain unless it’s your kink! (Rant)</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jlszqy/dont_pay_for_pain_unless_its_your_kink_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1jmgj2x</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Practicing shaping and filing my nails as a recovered nail-biter</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmgj2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1jmgg6j</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>One coaters ❤️</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmgg6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1jmg82r</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Storage feedback</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmg82r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1jmfrbe</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Sparkly copycat, sort of 😸</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oojb0l31ikre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1jmddlk</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Quitting dip powder, would like to transition to nail polish. Would like some support (:</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmddlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1jmd1g6</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Holo Taco Madness</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmd1g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1jmcnmb</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Help me get my hospital bound sister in order 🙏 (more below)</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3q5owhwkjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1jmchoq</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Wicked Skittle 🧹 🪄</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmchoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1jmbtzm</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Painted press ons, lasted twenty minutes before taking them off lol</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjg1y4eocjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1jmbs01</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Purple extravaganza! 💜💜</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpj3h2kicjre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1jmb0v4</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>I was a little nervous to try this one</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmb0v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1jmazpv</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Look Alive</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmazpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1jmaxfk</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Sunset sky skittle</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5c0iocn4jre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1jmahnp</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Glowier than expected</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmahnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1jma8sj</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>I can't believe I didn't think of this sooner✨️</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsebn10hyire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1jm9cvx</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>I just noticed that it says on the back that this is a gel polish. It is not marked as HEMA-free, but I think the ingredient list doesn't contain any of the allergens. Does this mean this might be okay, or are all gel polishes potential trouble?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zispb8k5qire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1jm8s0z</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>My 13 year old did her nails</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cci3t8zqlire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1jm86s4</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Did a crème mani, crème shows all sins</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm86s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1jm838s</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Everyone Deserves the Chance to Fly</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm838s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1jm7z7k</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Love the glow-in-the-dark polish + magnetic topper combo!</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm7z7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1jm7py6</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>am i using the wrong products?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jm7py6/am_i_using_the_wrong_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1jm7jue</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Update to EdM chipping!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm7jue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1jm6sha</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Random Dots?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm6sha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1jm6q94</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Flame Jelly (Candy Apple 🍎???)</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm6q94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1jm6obj</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>What was the strangest nail-related epiphany for you?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jm6obj/what_was_the_strangest_nailrelated_epiphany_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1jm6d07</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Day 14 vs day 1 (regular lacquer)</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm6d07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1jm67t3</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Cherry blossom blur</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9parxljv0ire1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1jm5ps2</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Hunger games inspired mani, just finished SOTR and I have a lot of emotions so this is my coping mechanism 😭</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm5ps2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1jm5o3b</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>It’s been 5 days and I just keep looking at my fingers</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nk2g69bmwhre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1jm5ank</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Subtle springy gradient</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm5ank</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1jm574a</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Sparkly coral combo</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm574a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1jm53i0</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Do all BKL collections come back for re-pours/overstock?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jm53i0/do_all_bkl_collections_come_back_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1jm51rp</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>See ya, Space Cowboy…</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm51rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1jm51a1</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>First Full Cracked Order! I’m so excited!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1z8krcurhre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1jm512s</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Obsessed with this color</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm512s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1jm50o8</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Limoncello by Le Mini Macaron with their short coffin nail extensions 💛</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm50o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1jm4qto</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Sweet Pea 🫛 Such a clean, refreshing, sparkly palate cleanser ✨</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u09f9jxkphre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1jm4n6a</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Stellar Evolution ✨️</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4n6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1jm4krt</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Mix it &amp; hope for the best (March franken &amp; layering compilation)</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4krt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1jm3lk7</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Another set inspired by Phos from Land of the Lustrous. There’s a whole character arc on my hands.</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm3lk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1jm3g5s</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Polish Pickup JuneTheme Voting is Open</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jm3g5s/polish_pickup_junetheme_voting_is_open/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1jm30n9</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>💅💅</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5ff2trfchre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1jlz347</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Transitioning to natural nails from builder gel?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlz347/transitioning_to_natural_nails_from_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1jm2mbq</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>I’m SO excited!! 😍</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcdv31mg9hre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1jm1zii</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Grabbed this polish in a mystery bag destash. Found out it has a fun surprise!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm1zii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1jm15u3</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Sprinkle Nail Design Feedback</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0cew6thygre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1jm0yls</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>I was influenced</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm0yls</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1jm0opj</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of this color?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm0opj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1jm0hwj</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>EXTREME SPARKLE</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f3qjnbahtgre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1jm00rz</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Mildly Interesting Thermal</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6dyghzxpgre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1jlztuf</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Emily de Molly Wished for Tomorrow</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlztuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1jlzp3a</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Apply nails and paint on separate days</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlzp3a/apply_nails_and_paint_on_separate_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1jlyiw8</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Work moisturizer hack</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kdc3q9ahegre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1jly0r2</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Spring Thaw</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jly0r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1jlxzo6</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>All Aglow🩵💛</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlxzo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1jlxwyw</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>This counts as a palette cleanser, right? (pics in comments)</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tm1rvh8t9gre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1jlxcl2</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Shimmery blue + new gems</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlxcl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1jlx4c3</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Enchanted To Meet You</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlx4c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1jlwicy</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Has anyone put the new BKL mosaic magnetics over black?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlwicy/has_anyone_put_the_new_bkl_mosaic_magnetics_over/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1jlwg7y</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Indomitable - 7 days in</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1meowyddyfre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1jlw8wq</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>I love the color shift!</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlw8wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1jlvjjp</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Base coat recommendations</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlvjjp/base_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1jlvfno</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>A tale of 2 manis</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlvfno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1jlv2fu</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Angel’s Breath over black ✨</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95fvl3rumfre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1jlugnj</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>I’m losing my mind</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha1b1l9lhfre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1jltzls</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Sally Hansen hard as nails</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jltzls/sally_hansen_hard_as_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1jlt1hv</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>My nails always split on the sides, so I keep having to cut them short. Any tips on having healthier nails?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jlt1hv/my_nails_always_split_on_the_sides_so_i_keep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1jl5xax</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Semi-portable polish storage solutions</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jl5xax/semiportable_polish_storage_solutions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1jl65xg</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>ISO Allergy Friendly Gel</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jl65xg/iso_allergy_friendly_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1jmgjuj</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Some of my fav nail sets</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmgjuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1jmg04r</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Just finished this set as a beginner. How’d I do? How can I improve?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmg04r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1jmfh0u</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Jelly nails</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jmfh0u/jelly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1jmf4jy</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>My first attempt at Easter egg nails 🐰🥚💅</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zygvomr3bkre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1jmc4r5</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Some of my nail art!✨</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmc4r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1jmbqc8</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>First time with jewelry</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cdsgihk2cjre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1jmbgej</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Not a very complex design but I did these little evil eyes for my second time ever trying DIY gel. Hoping to improve!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7cxm12j9jre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1jmaoe5</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Easter Nails</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmaoe5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1jm5rl4</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Hunger games inspired mani, just finished SOTR and I have a lot of emotions so this is my coping mechanism 😭</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm5rl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1jm55gc</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm55gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1jm557k</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfoae6unshre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1jm4pz0</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Bauhaus Movement inspired.</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm4pz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1jm1q1y</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Bohemian spring pedi</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm1q1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1jm0lqx</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Amantes del blanco 🤍🤍🤍</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uiec5uaugre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1jm0jn2</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Galaxy Nails 🌌</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jm0jn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1jlxh5p</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Cleaning nail stamper between stamps?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jlxh5p/cleaning_nail_stamper_between_stamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1jlxbqd</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>I always get to this point and decision paralysis sets in</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlxbqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1jlum6d</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Easter Nails 🫶</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqbu49evifre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1jluhcz</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0sgjuerhfre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1jluebt</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Cat eye and blooming gel</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxg5r200hfre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1jlu18i</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Custom press ons by me :)</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huxis0midfre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1jltfnr</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>🍒🌷🍒</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jltfnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1jls18a</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Nail doodles 📓</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofc5ic9urere1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1jlquuw</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Goth Glam 💅🏻 What do you think?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jlquuw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 30 08:10:01 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_30.xlsx
+++ b/data/collected_data/2025_03_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1278"/>
+  <dimension ref="A1:C1458"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22159,6 +22159,3066 @@
         </is>
       </c>
     </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1jn6pi9</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Why is there a gap between gel and my nail corners? Does it have to be there?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn6pi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1jn0knd</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Hi does anyone know?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn0knd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1jn0otc</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Why do my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nzm4xbp3qre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1jn4tyg</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Spring almond nails!!🥰</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn4tyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1jn4tv5</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Spring almond nails</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn4tv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1jn2gpf</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My spring inspired nails! Got my inspiration here! Thanks!</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3oc8j9gkqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1jn49pk</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Question about brittle nail care</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jn49pk/question_about_brittle_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1jn4jpb</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I didn’t know cat eye came in light shades before this week</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn4jpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1jn29tg</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>First time having pointed nails and using chrome powder.  Hands are with chrome, toes are natural without chrome. What a difference the chrome powder makes on original color.  Loving it.</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn29tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1jn3ode</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Spring blues 💕</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8bco5mtwqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1jn3n78</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Did princess peach nails for my wife.</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn3n78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1jn3bze</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>My nail girl is amazing</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abbmhjf6tqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1jn36b3</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Why is white considered a classy nail color?</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jn36b3/why_is_white_considered_a_classy_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1jn35fz</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Which nail polish remover do you prefer: acetone Vs non-acetone (ex: propylene carbonate)</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jn35fz/which_nail_polish_remover_do_you_prefer_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1jn34cx</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Gel x or natural?</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jn34cx/gel_x_or_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1jn2tz0</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Bananas and Buttons</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn2tz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1jn2gxg</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>my recent nail art using molding gel 🐍</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn2gxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1jn2emp</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>If you were to use acrylic paint in airbrush in a professional setting how would people view you?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jn2emp/if_you_were_to_use_acrylic_paint_in_airbrush_in_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1jn2dgz</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Transparent press ons?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8dk1c5kjqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1jn25ab</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>I love this color.</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iehygk8dhqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1jn1vlk</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Juicy pomegranate nails for Mexico 💦🍇🍒</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xotaopqeqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1jn1dsm</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Nail tech hooked me up today</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqzceeiy9qre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1jn0ub6</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>What can I expect from my first builder gel fill appointment?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn0ub6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1jn15jd</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>We're starting autumn in the Southern hemisphere! Here are my fall nails 🍂🍁 hope you like them!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn15jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1jn11fx</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Pretty basic but I started doing my own nails at home 🖤</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6b9siov6qre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1jn0ujd</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Trying to find a nail tech that does sculpted acrylics in bay area</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jn0ujd/trying_to_find_a_nail_tech_that_does_sculpted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1jn0pz4</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Nails for my cousins wedding</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnxkh8py3qre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1jn0j0x</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Chrome yellow nails!!</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn0j0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1jn0e2x</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Please convince me these aren’t too “flesh” coloured</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbgyfczz0qre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1jn00wx</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Celebrating spring with floral nail stickers!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi2tuk1nxpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1jn007v</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Beautiful</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsaua6vgxpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1jmzktz</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Colorful Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmzktz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1jmzh82</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>RAVE BAE</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmzh82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1jmzeqe</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>did my first set w design and charms , super happy w myself 🥰</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uw9hy6aspre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1jmz6x7</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Made the switch from a salon to a private nail tech and the results show for themselves</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmz6x7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1jmz3cx</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Loving this funky color 💚</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l1ab9njppre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1jmz3a3</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>China Glaze Boho Blues</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmz3a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1jmycgo</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Recent nails!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmycgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1jmxzmn</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>🙂</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br4wtrn4gpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1jmxyvw</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>slightly wild nails</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kb36p5kxfpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1jmxylm</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n02zo9kvfpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1jmxx8h</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>These were described as space fairy nails and I can’t think of anything better! 💫🧚</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmxx8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1jmxuv6</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Florals for spring? Groundbreaking 🌼</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wi38drkzepre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1jmxogf</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Love how these turned out🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zymvudgdpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1jmxo1l</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Brown forever baby</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wa0mb4bdpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1jmxljp</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>One of my fav sets I did on myselfff</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xreo87uqcpre1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1jmxj9h</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Butterfly season</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x095chd7cpre1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1jmxfqf</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>cat eyes !!</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plttiy5fbpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1jmx1d6</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Pretty in Pink</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8xbuu728pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1jmx8fa</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>spring nails!</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1manaoq9pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1jmx52o</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>So happy with my nails</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65k6450y8pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1jmx3o9</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Couldn't choose a color so went with all of them 😅</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkry48ul8pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1jmx14g</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Coquette nails</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmx14g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1jmww87</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Sage green spring nails</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmww87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1jmwvvl</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmwvvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1jmwvp5</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Warm weather is here!</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt57ocxq6pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1jmwtgw</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>a little flair for closing day 🏡</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6ljkpci06pre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1jmwrzw</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Curiosity of My Wife!</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmwrzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1jmwiab</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Is This a Good UV Lamp?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmwiab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1jmwenv</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Dried flowers for spring!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ll49w7p2pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1jmw4d2</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>What is going on here?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmw4d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1jmw3nr</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>How to have a long lasting mani with normal polish</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmw3nr/how_to_have_a_long_lasting_mani_with_normal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1jmw0wy</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Help??</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmw0wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1jmw1f8</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>My girlfriend doesn’t have Reddit so I thought I’d share her latest work here!! I love them. She’s a student a just started a couple months ago!</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmw1f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1jmvnzb</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>How did my bsf do for her 1st time?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmvnzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1jmvjo1</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>first time ever getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7oo8etkovore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1jmv6p0</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>The Cat Eye 😍</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmv6p0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1jmu2f0</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Press ons: Regular Glue or UV Gel?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmu2f0/press_ons_regular_glue_or_uv_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1jmuqds</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Berday Nails</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmuqds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1jmupq7</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>So happy with the shape &amp; colour this time ❣️</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmupq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1jmun4w</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>If I was a color I’d be chrome 💖</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpbc01tcoore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1jmugoz</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Spring naiiiils</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmugoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1jmufw7</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>I love my nails</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mhtj6ppmore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1jmtvo6</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Pink and green pedi</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmtvo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1jmss4k</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Nails for upcoming ARTMS concert</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmss4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1jmtc9h</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>press ons + top coat = ❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmtc9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1jmszcx</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmszcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1jmt3oc</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Dark Red ♥️💋🌹</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z9a14nobore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1jmspop</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Nails nails 💅</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93prqhwk8ore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1jmsilz</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>obsessed with the cateye!</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1m8slrp27ore1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1jmshi4</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Obsessed!!!!!!!</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8es9k51v6ore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1jms66c</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Sometimes a neat coat of polish is better than designs</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jms66c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1jms4an</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>I think biab comes off due to dehydration</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jms4an</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1jms7a9</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>ILNP - Jet Setter</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jms7a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1jmrvry</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Is there a name for this type of buffer/file?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmrvry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1jmrtf2</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Help I'm new to nails and confused about it</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmrtf2/help_im_new_to_nails_and_confused_about_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1jmrbyn</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmrbyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1jmhtz7</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Need to help my sister</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmhtz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1jminm4</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>First time trying to build with acrylic power</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8es21k2mlre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1jmjca0</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Gel polish brand recommendations that won’t break the bank?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2talbr4cvlre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1jmqxg4</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>🌷Spring nails🌷</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uypzhg2lunre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1jmqx8b</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>First time doing my own extensions - not just pressies!</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmqx8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1jmkwj0</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Is it better to get your nails done at a salon, or do them at home?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmkwj0/is_it_better_to_get_your_nails_done_at_a_salon_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1jmqg00</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Altar Ego Polish</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jmqg00/altar_ego_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1jmqilu</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Current situation...</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmqilu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1jmqay8</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Not sure if i did it correctly but it works :)</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmqay8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1jmq51j</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Getting your nails done is so therapeutic</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cz36rsconre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1jmq06y</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>fishing lure nails!!</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybluado9nnre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1jmpuh6</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Should I?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmeox0szlnre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1jmptfa</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>First time trying cat eye</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gifi2qvqlnre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1jn72qy</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Cirque jellies</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn72qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1jn5nen</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>PPU - what shades are being released?</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bghknn83jrre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1jn4fsb</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Glow in the Dark Flowers</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn4fsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1jn3vob</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Yup, it's another magnet post</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d7qjrmaxyqre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1jn2zv9</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>rainbow holo 🌈</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hk5ysjqpqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1jn2w88</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>What am I missing?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opye6mgqoqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1jn2knp</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Shoutout to Essie Good to Go</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn2knp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1jn2jot</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>This is ridiculous</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4szajtr9lqre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1jn2ir9</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>looking for a Nail Polish dupe for OPI funny bunny &amp; bubble bath GEL polish</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jn2ir9/looking_for_a_nail_polish_dupe_for_opi_funny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1jn2fbg</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Are some color shifts not possible?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jn2fbg/are_some_color_shifts_not_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1jn2bly</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Painting under clear press ons?</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn2bly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1jn1iz2</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Professional-looking French</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jn1iz2/professionallooking_french/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1jn18ri</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Butterfly Nail Art</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jn18ri/butterfly_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1jn111o</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Green version of Maelstrom?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jn111o/green_version_of_maelstrom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1jn0low</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Wildflower Lacquer Slug Bug 2.0: Sad about my press-ons, but happy about the polish!</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9v6e9vw2qre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1jn0ij3</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>top coat rec that doesn’t shrink?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jn0ij3/top_coat_rec_that_doesnt_shrink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1jmu4kb</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Current mani🍇</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71n57qgw0wqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1jmzipl</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Short coffin nails?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmzipl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1jmyrb3</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>PSA: Rainbow Connection will no longer be stocking Mooncat</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xndlhqfrmpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1jmyeyf</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>How to make my homemade mani look better</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmyeyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1jmy1a6</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Magnetic holo?</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nauocpqigpre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1jmxw8j</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Accidentally duped myself</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os1ei6pbfpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1jmxv6u</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Don’t you just ❤️ it when it comes together like that? 🫰🏼💥💙💚</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmxv6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1jmxdjq</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>My favorite magnetic lacquer 💙✨midnight sol</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mhzbtd1yapre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1jmx95b</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>I'm looking for a polish in this color</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmejdeax9pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1jmx71r</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Nails suddenly curving upwards?</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1h5orbse9pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1jmx3to</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Part 2!✨️</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhrypaom8pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1jmx2r1</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Spring rain</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgdge4id8pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1jmwjiu</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Such an opulent combo</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f465yezv3pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1jmweor</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>This lacquer combo gives me Barbie vibes</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmweor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1jmw58g</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Flower Child as a topper</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmw58g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1jmvubt</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Red and Black, Black and Red</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmvubt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1jmvebq</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Top coat ruined the holo?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfnidqrguore1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1jmv29a</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Mismatched Skittle Inspired by u/seyebird :)</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmv29a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1jmuvko</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>First “spring colored” mani of 2025</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmuvko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1jmuu7x</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>My first time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmuu7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1jmutoc</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>More magnetics?!?</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9q18bq3upore1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1jmumbf</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>first time trying arcana lacquers :)</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmumbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1jmum0c</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Having fun with layering</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmum0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1jmucqc</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Made a new friend</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic0dfnizlore1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1jmtmic</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Indomitable 💜</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmtmic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1jmtgaz</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Why do people like jellies?</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jmtgaz/why_do_people_like_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1jmt2r5</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>First Sassy Sauce order!</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmt2r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1jmsxtz</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>My Gecko Does Tricks by OPI dupe?</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jmsxtz/my_gecko_does_tricks_by_opi_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1jmsxri</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Tiffany blue dupe at Dollar Tree!</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqpjtyzeaore1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1jms7ve</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>ILNP - Jet Setter</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jms7ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1jms026</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Trying out a Canadian nail polish brand, order came in today and my daughter picked this colour to try out first (pink of course)</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jms026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1jmrwhp</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Decade of Decadence</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21yyix782ore1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1jmri9f</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Lavender Milk 💟</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmri9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1jmr6yg</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>What I wore this month</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmr6yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1jmqifk</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Cirque guabaya</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmqifk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1jmqczb</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>What is going on with my nails? White lines???</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh29lse4qnre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1jmq88s</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>La Petite Mort is stunning</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmq88s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1jmq7f8</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>First Jelly Sandwich: I’m in love</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yu5i2oawonre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1jmpcqr</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Tips on how to prevent tips chipping in 1 day?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmpcqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1jmpc93</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Getting back in the saddle</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0vmtvjwhnre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1jmonok</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Easy-open tip for Polish Boxes!</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmonok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1jmoi7o</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>It finally came!</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmoi7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1jmnj1g</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Help me pick spring colour</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmnj1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1jmn6eo</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Florals for spring? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmn6eo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1jmn64n</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Dabbling into magnetics again! Tried a magnetic multichrome skittle! 🌈🧲</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmn64n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1jmlufr</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Continuing the Spring vibes 🩵</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eim7jwgnnmre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1jmkcma</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>My first Cirque jelly: Morningtide</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8siacqu7mre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1jmk4ya</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Glowy crackle shatter 2.0</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmk4ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1jmin51</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Stars Above</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmin51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1jn5b8d</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Nails I did yesterday</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz8cmkv1frre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1jn3c6g</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>SpongeBob</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn3c6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1jn2sra</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Bananas and Buttons</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jn2sra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1jn1wdu</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Juicy pomegranate nails for Mexico done by @nails_emmywynn 💦🍇🍒</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sskdcbyeqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1jn1gg1</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Cat Eye Nails 💅</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2jmwzfnaqre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1jmytzc</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>First attempt at any sort of nail art :3</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0rjv3wcnpre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1jmy7k8</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>I have a question for those of you who do 3D art with sold gel.</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jmy7k8/i_have_a_question_for_those_of_you_who_do_3d_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1jmwx2d</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Amo el color verde</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7hr65827pre1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1jmtuvo</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Pink and green pedi</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmtuvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1jmsr6h</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Tried the butterfly trend and lowkey hate it 😭😭</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmsr6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1jmr63f</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>My attempt at the butterfly wing trend (had to cover up a horrible ombre attempt)</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmr63f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1jmlkh7</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Looking for Nail Tech in MA</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jmlkh7/looking_for_nail_tech_in_ma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1jmlfk1</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>This week's beach designs, which one is your favorite? 🌊🐙🏝️</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jmlfk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1jml60a</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Severance has taken over my life.</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jml60a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1jml2wh</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Spring set</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jml2wh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>